<commit_message>
added file from mail
</commit_message>
<xml_diff>
--- a/Chiffres  COVID-19 Valais.xlsx
+++ b/Chiffres  COVID-19 Valais.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\11. Maladies transmissibles\11.2. Lutte\11.2.3. Pandémies\COVID-19\Epi\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
@@ -24,7 +29,7 @@
     <author>Larissa VERNIER</author>
   </authors>
   <commentList>
-    <comment ref="D2" authorId="0">
+    <comment ref="D2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -94,16 +99,13 @@
     <t>Nb nouveaux décès extra-hospitaliers</t>
   </si>
   <si>
-    <t>Données COVID-19 Valais 06.05.2020</t>
-  </si>
-  <si>
-    <t>0</t>
+    <t>Données COVID-19 Valais 07.05.2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,7 +397,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -665,7 +667,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -676,23 +678,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O72"/>
+  <dimension ref="A1:O73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="11.42578125" style="15"/>
-    <col min="4" max="4" width="10.85546875" style="15"/>
-    <col min="8" max="8" width="16.140625" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" style="6" customWidth="1"/>
+    <col min="2" max="3" width="11.453125" style="15"/>
+    <col min="4" max="4" width="10.81640625" style="15"/>
+    <col min="8" max="8" width="16.1796875" customWidth="1"/>
+    <col min="10" max="10" width="14.54296875" customWidth="1"/>
+    <col min="11" max="11" width="13.54296875" customWidth="1"/>
+    <col min="12" max="12" width="15.7265625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="32" t="s">
         <v>13</v>
       </c>
@@ -708,7 +710,7 @@
       <c r="K1" s="33"/>
       <c r="L1" s="34"/>
     </row>
-    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -749,7 +751,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43889</v>
       </c>
@@ -791,7 +793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>43890</v>
       </c>
@@ -833,7 +835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>43891</v>
       </c>
@@ -875,7 +877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>43892</v>
       </c>
@@ -917,7 +919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>43893</v>
       </c>
@@ -959,7 +961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>43894</v>
       </c>
@@ -1001,7 +1003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>43895</v>
       </c>
@@ -1043,7 +1045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>43896</v>
       </c>
@@ -1085,7 +1087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>43897</v>
       </c>
@@ -1127,7 +1129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>43898</v>
       </c>
@@ -1169,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>43899</v>
       </c>
@@ -1211,7 +1213,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>43900</v>
       </c>
@@ -1253,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>43901</v>
       </c>
@@ -1295,7 +1297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>43902</v>
       </c>
@@ -1337,7 +1339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>43903</v>
       </c>
@@ -1379,7 +1381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>43904</v>
       </c>
@@ -1421,7 +1423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>43905</v>
       </c>
@@ -1463,7 +1465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>43906</v>
       </c>
@@ -1505,7 +1507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>43907</v>
       </c>
@@ -1547,7 +1549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>43908</v>
       </c>
@@ -1589,7 +1591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>43909</v>
       </c>
@@ -1631,7 +1633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>43910</v>
       </c>
@@ -1673,7 +1675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>43911</v>
       </c>
@@ -1715,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>43912</v>
       </c>
@@ -1757,7 +1759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>43913</v>
       </c>
@@ -1799,7 +1801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>43914</v>
       </c>
@@ -1841,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>43915</v>
       </c>
@@ -1883,7 +1885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>43916</v>
       </c>
@@ -1925,7 +1927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>43917</v>
       </c>
@@ -1967,7 +1969,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>43918</v>
       </c>
@@ -2009,7 +2011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>43919</v>
       </c>
@@ -2051,7 +2053,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>43920</v>
       </c>
@@ -2072,11 +2074,11 @@
         <v>23</v>
       </c>
       <c r="G34" s="24">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H34" s="17">
         <f t="shared" si="0"/>
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I34" s="16">
         <f t="shared" si="8"/>
@@ -2093,7 +2095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>43921</v>
       </c>
@@ -2114,11 +2116,11 @@
         <v>23</v>
       </c>
       <c r="G35" s="24">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H35" s="17">
         <f t="shared" ref="H35:H59" si="10">G35+E35</f>
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="I35" s="16">
         <f t="shared" si="8"/>
@@ -2135,7 +2137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>43922</v>
       </c>
@@ -2156,11 +2158,11 @@
         <v>25</v>
       </c>
       <c r="G36" s="24">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H36" s="17">
         <f t="shared" si="10"/>
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I36" s="16">
         <f t="shared" si="8"/>
@@ -2177,7 +2179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>43923</v>
       </c>
@@ -2198,11 +2200,11 @@
         <v>24</v>
       </c>
       <c r="G37" s="24">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H37" s="17">
         <f t="shared" si="10"/>
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I37" s="16">
         <f t="shared" si="8"/>
@@ -2219,7 +2221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>43924</v>
       </c>
@@ -2240,11 +2242,11 @@
         <v>23</v>
       </c>
       <c r="G38" s="24">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H38" s="17">
         <f t="shared" si="10"/>
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I38" s="16">
         <f t="shared" si="8"/>
@@ -2261,7 +2263,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>43925</v>
       </c>
@@ -2282,11 +2284,11 @@
         <v>23</v>
       </c>
       <c r="G39" s="24">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H39" s="17">
         <f t="shared" si="10"/>
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="I39" s="16">
         <f t="shared" si="8"/>
@@ -2303,7 +2305,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>43926</v>
       </c>
@@ -2324,11 +2326,11 @@
         <v>23</v>
       </c>
       <c r="G40" s="24">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H40" s="17">
         <f t="shared" si="10"/>
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="I40" s="16">
         <f t="shared" si="8"/>
@@ -2345,7 +2347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>43927</v>
       </c>
@@ -2366,11 +2368,11 @@
         <v>22</v>
       </c>
       <c r="G41" s="24">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H41" s="17">
         <f t="shared" si="10"/>
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="I41" s="16">
         <f t="shared" si="8"/>
@@ -2387,7 +2389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>43928</v>
       </c>
@@ -2408,11 +2410,11 @@
         <v>20</v>
       </c>
       <c r="G42" s="24">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H42" s="17">
         <f t="shared" si="10"/>
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I42" s="16">
         <f t="shared" si="8"/>
@@ -2429,7 +2431,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>43929</v>
       </c>
@@ -2450,11 +2452,11 @@
         <v>20</v>
       </c>
       <c r="G43" s="24">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H43" s="17">
         <f t="shared" si="10"/>
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I43" s="16">
         <f t="shared" si="8"/>
@@ -2471,7 +2473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>43930</v>
       </c>
@@ -2492,11 +2494,11 @@
         <v>19</v>
       </c>
       <c r="G44" s="24">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H44" s="17">
         <f t="shared" si="10"/>
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="I44" s="16">
         <f t="shared" si="8"/>
@@ -2513,7 +2515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43931</v>
       </c>
@@ -2534,11 +2536,11 @@
         <v>18</v>
       </c>
       <c r="G45" s="24">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H45" s="17">
         <f t="shared" si="10"/>
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="I45" s="16">
         <f t="shared" si="8"/>
@@ -2555,7 +2557,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>43932</v>
       </c>
@@ -2576,11 +2578,11 @@
         <v>15</v>
       </c>
       <c r="G46" s="24">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H46" s="17">
         <f t="shared" si="10"/>
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I46" s="16">
         <f t="shared" si="8"/>
@@ -2597,7 +2599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>43933</v>
       </c>
@@ -2618,11 +2620,11 @@
         <v>14</v>
       </c>
       <c r="G47" s="24">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H47" s="17">
         <f t="shared" si="10"/>
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I47" s="16">
         <f t="shared" si="8"/>
@@ -2639,7 +2641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>43934</v>
       </c>
@@ -2660,11 +2662,11 @@
         <v>12</v>
       </c>
       <c r="G48" s="24">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H48" s="17">
         <f t="shared" si="10"/>
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I48" s="16">
         <f t="shared" si="8"/>
@@ -2681,7 +2683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>43935</v>
       </c>
@@ -2702,11 +2704,11 @@
         <v>11</v>
       </c>
       <c r="G49" s="24">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H49" s="17">
         <f t="shared" si="10"/>
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I49" s="16">
         <f t="shared" si="8"/>
@@ -2723,7 +2725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>43936</v>
       </c>
@@ -2744,11 +2746,11 @@
         <v>12</v>
       </c>
       <c r="G50" s="24">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H50" s="17">
         <f t="shared" si="10"/>
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I50" s="16">
         <f t="shared" si="8"/>
@@ -2765,7 +2767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>43937</v>
       </c>
@@ -2786,11 +2788,11 @@
         <v>12</v>
       </c>
       <c r="G51" s="24">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H51" s="17">
         <f t="shared" si="10"/>
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I51" s="16">
         <f t="shared" si="8"/>
@@ -2807,7 +2809,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>43938</v>
       </c>
@@ -2828,11 +2830,11 @@
         <v>10</v>
       </c>
       <c r="G52" s="24">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H52" s="17">
         <f t="shared" si="10"/>
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="I52" s="16">
         <f t="shared" si="8"/>
@@ -2849,7 +2851,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>43939</v>
       </c>
@@ -2870,11 +2872,11 @@
         <v>10</v>
       </c>
       <c r="G53" s="24">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H53" s="17">
         <f t="shared" si="10"/>
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="I53" s="16">
         <f t="shared" si="8"/>
@@ -2891,7 +2893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>43940</v>
       </c>
@@ -2912,11 +2914,11 @@
         <v>9</v>
       </c>
       <c r="G54" s="24">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H54" s="17">
         <f t="shared" si="10"/>
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I54" s="16">
         <f t="shared" si="8"/>
@@ -2933,7 +2935,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>43941</v>
       </c>
@@ -2954,11 +2956,11 @@
         <v>9</v>
       </c>
       <c r="G55" s="24">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H55" s="17">
         <f t="shared" si="10"/>
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="I55" s="16">
         <f t="shared" si="8"/>
@@ -2975,7 +2977,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>43942</v>
       </c>
@@ -2996,11 +2998,11 @@
         <v>10</v>
       </c>
       <c r="G56" s="24">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H56" s="17">
         <f t="shared" si="10"/>
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="I56" s="16">
         <f t="shared" ref="I56:I59" si="12">I55+J56</f>
@@ -3017,7 +3019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>43943</v>
       </c>
@@ -3038,11 +3040,11 @@
         <v>10</v>
       </c>
       <c r="G57" s="24">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="H57" s="17">
         <f t="shared" si="10"/>
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="I57" s="16">
         <f t="shared" si="12"/>
@@ -3059,7 +3061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>43944</v>
       </c>
@@ -3080,11 +3082,11 @@
         <v>9</v>
       </c>
       <c r="G58" s="24">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H58" s="17">
         <f t="shared" si="10"/>
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I58" s="16">
         <f t="shared" si="12"/>
@@ -3101,7 +3103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>43945</v>
       </c>
@@ -3122,11 +3124,11 @@
         <v>9</v>
       </c>
       <c r="G59" s="24">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H59" s="17">
         <f t="shared" si="10"/>
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I59" s="16">
         <f t="shared" si="12"/>
@@ -3143,7 +3145,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>43946</v>
       </c>
@@ -3164,11 +3166,11 @@
         <v>9</v>
       </c>
       <c r="G60" s="24">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H60" s="17">
         <f t="shared" ref="H60:H63" si="15">G60+E60</f>
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I60" s="16">
         <f t="shared" ref="I60:I63" si="16">I59+J60</f>
@@ -3185,7 +3187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>43947</v>
       </c>
@@ -3206,11 +3208,11 @@
         <v>8</v>
       </c>
       <c r="G61" s="24">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H61" s="17">
         <f t="shared" si="15"/>
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I61" s="16">
         <f t="shared" si="16"/>
@@ -3227,7 +3229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>43948</v>
       </c>
@@ -3248,11 +3250,11 @@
         <v>9</v>
       </c>
       <c r="G62" s="24">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H62" s="17">
         <f t="shared" si="15"/>
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="I62" s="16">
         <f t="shared" si="16"/>
@@ -3269,7 +3271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>43949</v>
       </c>
@@ -3290,11 +3292,11 @@
         <v>8</v>
       </c>
       <c r="G63" s="24">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H63" s="17">
         <f t="shared" si="15"/>
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="I63" s="16">
         <f t="shared" si="16"/>
@@ -3311,12 +3313,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>43950</v>
       </c>
       <c r="B64" s="19">
-        <f t="shared" ref="B64:B70" si="18">B63+C64</f>
+        <f t="shared" ref="B64:B66" si="18">B63+C64</f>
         <v>1876</v>
       </c>
       <c r="C64" s="13">
@@ -3332,18 +3334,18 @@
         <v>8</v>
       </c>
       <c r="G64" s="24">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H64" s="17">
-        <f t="shared" ref="H64:H71" si="19">G64+E64</f>
-        <v>61</v>
+        <f t="shared" ref="H64:H66" si="19">G64+E64</f>
+        <v>62</v>
       </c>
       <c r="I64" s="16">
-        <f t="shared" ref="I64:I71" si="20">I63+J64</f>
+        <f t="shared" ref="I64:I66" si="20">I63+J64</f>
         <v>136</v>
       </c>
       <c r="J64" s="16">
-        <f t="shared" ref="J64:J71" si="21">K64+L64</f>
+        <f t="shared" ref="J64:J66" si="21">K64+L64</f>
         <v>1</v>
       </c>
       <c r="K64" s="26">
@@ -3353,7 +3355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>43951</v>
       </c>
@@ -3374,11 +3376,11 @@
         <v>8</v>
       </c>
       <c r="G65" s="24">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H65" s="17">
         <f t="shared" si="19"/>
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I65" s="16">
         <f t="shared" si="20"/>
@@ -3395,16 +3397,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>43952</v>
       </c>
       <c r="B66" s="19">
         <f t="shared" si="18"/>
-        <v>1886</v>
+        <v>1887</v>
       </c>
       <c r="C66" s="13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D66" s="13">
         <v>0</v>
@@ -3416,11 +3418,11 @@
         <v>8</v>
       </c>
       <c r="G66" s="24">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H66" s="17">
         <f t="shared" si="19"/>
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="I66" s="16">
         <f t="shared" si="20"/>
@@ -3437,13 +3439,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>43953</v>
       </c>
       <c r="B67" s="19">
-        <f t="shared" si="18"/>
-        <v>1888</v>
+        <f t="shared" ref="B67:B71" si="22">B66+C67</f>
+        <v>1889</v>
       </c>
       <c r="C67" s="13">
         <v>2</v>
@@ -3458,18 +3460,18 @@
         <v>8</v>
       </c>
       <c r="G67" s="24">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H67" s="17">
-        <f t="shared" si="19"/>
-        <v>59</v>
+        <f t="shared" ref="H67:H72" si="23">G67+E67</f>
+        <v>60</v>
       </c>
       <c r="I67" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="I67:I72" si="24">I66+J67</f>
         <v>140</v>
       </c>
       <c r="J67" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="J67:J72" si="25">K67+L67</f>
         <v>2</v>
       </c>
       <c r="K67" s="26">
@@ -3479,13 +3481,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>43954</v>
       </c>
       <c r="B68" s="19">
-        <f t="shared" si="18"/>
-        <v>1890</v>
+        <f t="shared" si="22"/>
+        <v>1891</v>
       </c>
       <c r="C68" s="13">
         <v>2</v>
@@ -3500,18 +3502,18 @@
         <v>8</v>
       </c>
       <c r="G68" s="24">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H68" s="17">
-        <f t="shared" si="19"/>
-        <v>59</v>
+        <f t="shared" si="23"/>
+        <v>60</v>
       </c>
       <c r="I68" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>142</v>
       </c>
       <c r="J68" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>2</v>
       </c>
       <c r="K68" s="26">
@@ -3521,16 +3523,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>43955</v>
       </c>
       <c r="B69" s="19">
-        <f t="shared" si="18"/>
-        <v>1897</v>
+        <f t="shared" si="22"/>
+        <v>1899</v>
       </c>
       <c r="C69" s="13">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D69" s="13">
         <v>0</v>
@@ -3542,18 +3544,18 @@
         <v>7</v>
       </c>
       <c r="G69" s="24">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H69" s="17">
-        <f t="shared" si="19"/>
-        <v>54</v>
+        <f t="shared" si="23"/>
+        <v>55</v>
       </c>
       <c r="I69" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>142</v>
       </c>
       <c r="J69" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K69" s="26">
@@ -3563,13 +3565,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>43956</v>
       </c>
       <c r="B70" s="19">
-        <f t="shared" si="18"/>
-        <v>1897</v>
+        <f t="shared" si="22"/>
+        <v>1899</v>
       </c>
       <c r="C70" s="13">
         <v>0</v>
@@ -3584,18 +3586,18 @@
         <v>6</v>
       </c>
       <c r="G70" s="24">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H70" s="17">
-        <f t="shared" si="19"/>
-        <v>49</v>
+        <f t="shared" si="23"/>
+        <v>50</v>
       </c>
       <c r="I70" s="16">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>146</v>
       </c>
       <c r="J70" s="16">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>4</v>
       </c>
       <c r="K70" s="26">
@@ -3605,45 +3607,87 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="2">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A71" s="1">
         <v>43957</v>
       </c>
-      <c r="B71" s="20"/>
-      <c r="C71" s="14"/>
-      <c r="D71" s="14">
-        <v>0</v>
-      </c>
-      <c r="E71" s="30">
+      <c r="B71" s="19">
+        <f t="shared" si="22"/>
+        <v>1899</v>
+      </c>
+      <c r="C71" s="13">
+        <v>0</v>
+      </c>
+      <c r="D71" s="13">
+        <v>0</v>
+      </c>
+      <c r="E71" s="4">
         <v>8</v>
       </c>
-      <c r="F71" s="31">
-        <v>6</v>
-      </c>
-      <c r="G71" s="25">
-        <v>41</v>
-      </c>
-      <c r="H71" s="18">
-        <f t="shared" si="19"/>
-        <v>49</v>
-      </c>
-      <c r="I71" s="21">
-        <f t="shared" si="20"/>
+      <c r="F71" s="3">
+        <v>5</v>
+      </c>
+      <c r="G71" s="24">
+        <v>39</v>
+      </c>
+      <c r="H71" s="17">
+        <f t="shared" si="23"/>
+        <v>47</v>
+      </c>
+      <c r="I71" s="16">
+        <f t="shared" si="24"/>
         <v>146</v>
       </c>
-      <c r="J71" s="21">
-        <f t="shared" si="21"/>
-        <v>0</v>
-      </c>
-      <c r="K71" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="L71" s="29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F72" t="s">
+      <c r="J71" s="16">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="K71" s="26">
+        <v>0</v>
+      </c>
+      <c r="L71" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A72" s="2">
+        <v>43958</v>
+      </c>
+      <c r="B72" s="20"/>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14">
+        <v>0</v>
+      </c>
+      <c r="E72" s="30">
+        <v>9</v>
+      </c>
+      <c r="F72" s="31">
+        <v>5</v>
+      </c>
+      <c r="G72" s="25">
+        <v>38</v>
+      </c>
+      <c r="H72" s="18">
+        <f t="shared" si="23"/>
+        <v>47</v>
+      </c>
+      <c r="I72" s="21">
+        <f t="shared" si="24"/>
+        <v>146</v>
+      </c>
+      <c r="J72" s="21">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="K72" s="28">
+        <v>0</v>
+      </c>
+      <c r="L72" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F73" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added File for today from e-mail
</commit_message>
<xml_diff>
--- a/Chiffres  COVID-19 Valais.xlsx
+++ b/Chiffres  COVID-19 Valais.xlsx
@@ -99,7 +99,7 @@
     <t>Nb nouveaux décès extra-hospitaliers</t>
   </si>
   <si>
-    <t>Données COVID-19 Valais 07.05.2020</t>
+    <t>Données COVID-19 Valais 08.05.2020</t>
   </si>
 </sst>
 </file>
@@ -678,10 +678,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O73"/>
+  <dimension ref="A1:O74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L1"/>
+    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3361,10 +3361,10 @@
       </c>
       <c r="B65" s="19">
         <f t="shared" si="18"/>
-        <v>1882</v>
+        <v>1883</v>
       </c>
       <c r="C65" s="13">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D65" s="13">
         <v>1</v>
@@ -3403,7 +3403,7 @@
       </c>
       <c r="B66" s="19">
         <f t="shared" si="18"/>
-        <v>1887</v>
+        <v>1888</v>
       </c>
       <c r="C66" s="13">
         <v>5</v>
@@ -3445,10 +3445,10 @@
       </c>
       <c r="B67" s="19">
         <f t="shared" ref="B67:B71" si="22">B66+C67</f>
-        <v>1889</v>
+        <v>1891</v>
       </c>
       <c r="C67" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D67" s="13">
         <v>2</v>
@@ -3463,15 +3463,15 @@
         <v>50</v>
       </c>
       <c r="H67" s="17">
-        <f t="shared" ref="H67:H72" si="23">G67+E67</f>
+        <f t="shared" ref="H67:H73" si="23">G67+E67</f>
         <v>60</v>
       </c>
       <c r="I67" s="16">
-        <f t="shared" ref="I67:I72" si="24">I66+J67</f>
+        <f t="shared" ref="I67:I71" si="24">I66+J67</f>
         <v>140</v>
       </c>
       <c r="J67" s="16">
-        <f t="shared" ref="J67:J72" si="25">K67+L67</f>
+        <f t="shared" ref="J67:J73" si="25">K67+L67</f>
         <v>2</v>
       </c>
       <c r="K67" s="26">
@@ -3487,7 +3487,7 @@
       </c>
       <c r="B68" s="19">
         <f t="shared" si="22"/>
-        <v>1891</v>
+        <v>1893</v>
       </c>
       <c r="C68" s="13">
         <v>2</v>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="B69" s="19">
         <f t="shared" si="22"/>
-        <v>1899</v>
+        <v>1901</v>
       </c>
       <c r="C69" s="13">
         <v>8</v>
@@ -3571,10 +3571,10 @@
       </c>
       <c r="B70" s="19">
         <f t="shared" si="22"/>
-        <v>1899</v>
+        <v>1903</v>
       </c>
       <c r="C70" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D70" s="13">
         <v>0</v>
@@ -3613,10 +3613,10 @@
       </c>
       <c r="B71" s="19">
         <f t="shared" si="22"/>
-        <v>1899</v>
+        <v>1905</v>
       </c>
       <c r="C71" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D71" s="13">
         <v>0</v>
@@ -3650,44 +3650,86 @@
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A72" s="2">
+      <c r="A72" s="1">
         <v>43958</v>
       </c>
-      <c r="B72" s="20"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14">
-        <v>0</v>
-      </c>
-      <c r="E72" s="30">
-        <v>9</v>
-      </c>
-      <c r="F72" s="31">
+      <c r="B72" s="19">
+        <f t="shared" ref="B72:B73" si="26">B71+C72</f>
+        <v>1905</v>
+      </c>
+      <c r="C72" s="13">
+        <v>0</v>
+      </c>
+      <c r="D72" s="13">
+        <v>0</v>
+      </c>
+      <c r="E72" s="4">
+        <v>8</v>
+      </c>
+      <c r="F72" s="3">
         <v>5</v>
       </c>
-      <c r="G72" s="25">
-        <v>38</v>
-      </c>
-      <c r="H72" s="18">
-        <f t="shared" si="23"/>
-        <v>47</v>
-      </c>
-      <c r="I72" s="21">
-        <f t="shared" si="24"/>
+      <c r="G72" s="24">
+        <v>34</v>
+      </c>
+      <c r="H72" s="17">
+        <f t="shared" ref="H72:H73" si="27">G72+E72</f>
+        <v>42</v>
+      </c>
+      <c r="I72" s="16">
+        <f t="shared" ref="I72:I73" si="28">I71+J72</f>
         <v>146</v>
       </c>
-      <c r="J72" s="21">
-        <f t="shared" si="25"/>
-        <v>0</v>
-      </c>
-      <c r="K72" s="28">
-        <v>0</v>
-      </c>
-      <c r="L72" s="29">
+      <c r="J72" s="16">
+        <f t="shared" ref="J72:J73" si="29">K72+L72</f>
+        <v>0</v>
+      </c>
+      <c r="K72" s="26">
+        <v>0</v>
+      </c>
+      <c r="L72" s="27">
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="F73" t="s">
+      <c r="A73" s="2">
+        <v>43959</v>
+      </c>
+      <c r="B73" s="20"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14">
+        <v>0</v>
+      </c>
+      <c r="E73" s="30">
+        <v>8</v>
+      </c>
+      <c r="F73" s="31">
+        <v>5</v>
+      </c>
+      <c r="G73" s="25">
+        <v>33</v>
+      </c>
+      <c r="H73" s="18">
+        <f t="shared" si="27"/>
+        <v>41</v>
+      </c>
+      <c r="I73" s="21">
+        <f t="shared" si="28"/>
+        <v>146</v>
+      </c>
+      <c r="J73" s="21">
+        <f t="shared" si="29"/>
+        <v>0</v>
+      </c>
+      <c r="K73" s="28">
+        <v>0</v>
+      </c>
+      <c r="L73" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="F74" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added file for today
</commit_message>
<xml_diff>
--- a/Chiffres  COVID-19 Valais.xlsx
+++ b/Chiffres  COVID-19 Valais.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Jidfs\users\B105PLS\Documents\COVID-Monitoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\11. Maladies transmissibles\11.2. Lutte\11.2.3. Pandémies\COVID-19\Epi\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -96,7 +96,7 @@
     <t>Nb nouveaux décès extra-hospitaliers</t>
   </si>
   <si>
-    <t>Données COVID-19 Valais 18.05.2020</t>
+    <t>Données COVID-19 Valais 19.05.2020</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -410,7 +410,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -675,23 +675,23 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O83"/>
+  <dimension ref="A1:O84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D94" sqref="D94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="11.453125" style="15"/>
-    <col min="4" max="4" width="10.81640625" style="15"/>
-    <col min="8" max="8" width="16.1796875" customWidth="1"/>
-    <col min="10" max="10" width="14.54296875" customWidth="1"/>
-    <col min="11" max="11" width="13.54296875" customWidth="1"/>
-    <col min="12" max="12" width="15.7265625" style="6" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" style="15"/>
+    <col min="4" max="4" width="10.85546875" style="15"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>12</v>
       </c>
@@ -707,7 +707,7 @@
       <c r="K1" s="33"/>
       <c r="L1" s="34"/>
     </row>
-    <row r="2" spans="1:15" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
@@ -748,7 +748,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43889</v>
       </c>
@@ -790,7 +790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43890</v>
       </c>
@@ -832,7 +832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43891</v>
       </c>
@@ -874,7 +874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43892</v>
       </c>
@@ -916,7 +916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43893</v>
       </c>
@@ -958,7 +958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43894</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43895</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43896</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43897</v>
       </c>
@@ -1126,7 +1126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43898</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43899</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43900</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43901</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43902</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43903</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43904</v>
       </c>
@@ -1420,7 +1420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43905</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43906</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43907</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43908</v>
       </c>
@@ -1588,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43909</v>
       </c>
@@ -1630,7 +1630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43910</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43911</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43912</v>
       </c>
@@ -1756,7 +1756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43913</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43914</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43915</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43916</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43917</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43918</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43919</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43920</v>
       </c>
@@ -2092,7 +2092,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43921</v>
       </c>
@@ -2134,7 +2134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43922</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43923</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43924</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43925</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43926</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43927</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43928</v>
       </c>
@@ -2428,7 +2428,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43929</v>
       </c>
@@ -2470,7 +2470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43930</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43931</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43932</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43933</v>
       </c>
@@ -2638,7 +2638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43934</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43935</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43936</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43937</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43938</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43939</v>
       </c>
@@ -2890,7 +2890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43940</v>
       </c>
@@ -2932,7 +2932,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43941</v>
       </c>
@@ -2974,7 +2974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43942</v>
       </c>
@@ -3016,7 +3016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43943</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43944</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43945</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43946</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43947</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43948</v>
       </c>
@@ -3268,7 +3268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43949</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43950</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>43951</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>43952</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>43953</v>
       </c>
@@ -3478,7 +3478,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>43954</v>
       </c>
@@ -3520,7 +3520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>43955</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>43956</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>43957</v>
       </c>
@@ -3646,12 +3646,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>43958</v>
       </c>
       <c r="B72" s="19">
-        <f t="shared" ref="B72:B82" si="14">B71+C72</f>
+        <f t="shared" ref="B72:B83" si="14">B71+C72</f>
         <v>1907</v>
       </c>
       <c r="C72" s="13">
@@ -3670,15 +3670,15 @@
         <v>36</v>
       </c>
       <c r="H72" s="17">
-        <f t="shared" ref="H72:H83" si="15">G72+E72</f>
+        <f t="shared" ref="H72:H84" si="15">G72+E72</f>
         <v>44</v>
       </c>
       <c r="I72" s="16">
-        <f t="shared" ref="I72:I83" si="16">I71+J72</f>
+        <f t="shared" ref="I72:I84" si="16">I71+J72</f>
         <v>146</v>
       </c>
       <c r="J72" s="16">
-        <f t="shared" ref="J72:J83" si="17">K72+L72</f>
+        <f t="shared" ref="J72:J84" si="17">K72+L72</f>
         <v>0</v>
       </c>
       <c r="K72" s="26">
@@ -3688,7 +3688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>43959</v>
       </c>
@@ -3730,7 +3730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>43960</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>43961</v>
       </c>
@@ -3814,7 +3814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>43962</v>
       </c>
@@ -3856,7 +3856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>43963</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>43964</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>43965</v>
       </c>
@@ -3982,12 +3982,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>43966</v>
       </c>
       <c r="B80" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="B80:B84" si="18">B79+C80</f>
         <v>1928</v>
       </c>
       <c r="C80" s="13">
@@ -4006,15 +4006,15 @@
         <v>24</v>
       </c>
       <c r="H80" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" ref="H80:H84" si="19">G80+E80</f>
         <v>31</v>
       </c>
       <c r="I80" s="16">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="I80:I84" si="20">I79+J80</f>
         <v>149</v>
       </c>
       <c r="J80" s="16">
-        <f t="shared" si="17"/>
+        <f t="shared" ref="J80:J84" si="21">K80+L80</f>
         <v>0</v>
       </c>
       <c r="K80" s="26">
@@ -4024,12 +4024,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>43967</v>
       </c>
       <c r="B81" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1931</v>
       </c>
       <c r="C81" s="13">
@@ -4048,15 +4048,15 @@
         <v>24</v>
       </c>
       <c r="H81" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>31</v>
       </c>
       <c r="I81" s="16">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>149</v>
       </c>
       <c r="J81" s="16">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K81" s="26">
@@ -4066,12 +4066,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>43968</v>
       </c>
       <c r="B82" s="19">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>1931</v>
       </c>
       <c r="C82" s="13">
@@ -4090,15 +4090,15 @@
         <v>24</v>
       </c>
       <c r="H82" s="17">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>31</v>
       </c>
       <c r="I82" s="16">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>149</v>
       </c>
       <c r="J82" s="16">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K82" s="26">
@@ -4108,40 +4108,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A83" s="2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
         <v>43969</v>
       </c>
-      <c r="B83" s="20"/>
-      <c r="C83" s="14"/>
-      <c r="D83" s="14">
-        <v>0</v>
-      </c>
-      <c r="E83" s="30">
+      <c r="B83" s="19">
+        <f t="shared" si="18"/>
+        <v>1932</v>
+      </c>
+      <c r="C83" s="13">
+        <v>1</v>
+      </c>
+      <c r="D83" s="13">
+        <v>1</v>
+      </c>
+      <c r="E83" s="4">
         <v>6</v>
       </c>
-      <c r="F83" s="31">
+      <c r="F83" s="3">
         <v>4</v>
       </c>
-      <c r="G83" s="25">
-        <v>24</v>
-      </c>
-      <c r="H83" s="18">
-        <f t="shared" si="15"/>
-        <v>30</v>
-      </c>
-      <c r="I83" s="21">
-        <f t="shared" si="16"/>
-        <v>150</v>
-      </c>
-      <c r="J83" s="21">
-        <f t="shared" si="17"/>
-        <v>1</v>
-      </c>
-      <c r="K83" s="28">
-        <v>1</v>
-      </c>
-      <c r="L83" s="29">
+      <c r="G83" s="24">
+        <v>23</v>
+      </c>
+      <c r="H83" s="17">
+        <f t="shared" si="19"/>
+        <v>29</v>
+      </c>
+      <c r="I83" s="16">
+        <f t="shared" si="20"/>
+        <v>151</v>
+      </c>
+      <c r="J83" s="16">
+        <f t="shared" si="21"/>
+        <v>2</v>
+      </c>
+      <c r="K83" s="26">
+        <v>1</v>
+      </c>
+      <c r="L83" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>43970</v>
+      </c>
+      <c r="B84" s="20">
+        <f t="shared" si="18"/>
+        <v>1933</v>
+      </c>
+      <c r="C84" s="14">
+        <v>1</v>
+      </c>
+      <c r="D84" s="14">
+        <v>0</v>
+      </c>
+      <c r="E84" s="30">
+        <v>6</v>
+      </c>
+      <c r="F84" s="31">
+        <v>4</v>
+      </c>
+      <c r="G84" s="25">
+        <v>23</v>
+      </c>
+      <c r="H84" s="18">
+        <f t="shared" si="19"/>
+        <v>29</v>
+      </c>
+      <c r="I84" s="21">
+        <f t="shared" si="20"/>
+        <v>151</v>
+      </c>
+      <c r="J84" s="21">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="K84" s="28">
+        <v>0</v>
+      </c>
+      <c r="L84" s="29">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
remove values for the 28.10.2020
</commit_message>
<xml_diff>
--- a/Chiffres  COVID-19 Valais.xlsx
+++ b/Chiffres  COVID-19 Valais.xlsx
@@ -696,10 +696,10 @@
   <dimension ref="A1:M310"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B228" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B222" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E246" sqref="E246"/>
+      <selection pane="bottomRight" activeCell="F247" sqref="F247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11709,30 +11709,16 @@
       <c r="A246" s="1">
         <v>44132</v>
       </c>
-      <c r="B246" s="13">
-        <f t="shared" ca="1" si="16"/>
-        <v>9853</v>
-      </c>
+      <c r="B246" s="13"/>
       <c r="C246" s="34"/>
-      <c r="D246" s="7">
-        <v>0</v>
-      </c>
+      <c r="D246" s="7"/>
       <c r="E246" s="3"/>
       <c r="F246" s="26"/>
       <c r="G246" s="16"/>
-      <c r="H246" s="11">
-        <f t="shared" ca="1" si="17"/>
-        <v>0</v>
-      </c>
+      <c r="H246" s="11"/>
       <c r="I246" s="24"/>
-      <c r="J246" s="10">
-        <f t="shared" ca="1" si="18"/>
-        <v>198</v>
-      </c>
-      <c r="K246" s="10">
-        <f t="shared" ca="1" si="19"/>
-        <v>0</v>
-      </c>
+      <c r="J246" s="10"/>
+      <c r="K246" s="10"/>
       <c r="L246" s="18"/>
       <c r="M246" s="19"/>
     </row>

</xml_diff>